<commit_message>
minor changes to readme and the excel file
</commit_message>
<xml_diff>
--- a/carbide_expansion_april2024.xlsx
+++ b/carbide_expansion_april2024.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="120">
   <si>
     <t>Metadata</t>
   </si>
@@ -339,9 +339,6 @@
   </si>
   <si>
     <t>estimated compressive ductility</t>
-  </si>
-  <si>
-    <t>&gt;50</t>
   </si>
   <si>
     <t>T4</t>
@@ -2337,8 +2334,8 @@
       <c r="I17" s="81">
         <v>298</v>
       </c>
-      <c r="J17" s="82" t="s">
-        <v>78</v>
+      <c r="J17" s="82">
+        <v>50</v>
       </c>
       <c r="K17" s="83"/>
       <c r="L17" s="77" t="s">
@@ -2575,7 +2572,7 @@
         <v>33</v>
       </c>
       <c r="M22" s="77" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N22" s="77" t="s">
         <v>69</v>
@@ -2621,7 +2618,7 @@
         <v>33</v>
       </c>
       <c r="M23" s="77" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N23" s="77" t="s">
         <v>69</v>
@@ -2667,7 +2664,7 @@
         <v>33</v>
       </c>
       <c r="M24" s="77" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N24" s="77" t="s">
         <v>69</v>
@@ -2713,7 +2710,7 @@
         <v>33</v>
       </c>
       <c r="M25" s="77" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N25" s="77" t="s">
         <v>69</v>
@@ -2759,7 +2756,7 @@
         <v>33</v>
       </c>
       <c r="M26" s="77" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N26" s="77" t="s">
         <v>69</v>
@@ -2805,7 +2802,7 @@
         <v>33</v>
       </c>
       <c r="M27" s="77" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N27" s="77" t="s">
         <v>69</v>
@@ -2851,7 +2848,7 @@
         <v>33</v>
       </c>
       <c r="M28" s="77" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N28" s="77" t="s">
         <v>69</v>
@@ -2897,7 +2894,7 @@
         <v>33</v>
       </c>
       <c r="M29" s="77" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N29" s="77" t="s">
         <v>69</v>
@@ -2943,7 +2940,7 @@
         <v>33</v>
       </c>
       <c r="M30" s="77" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N30" s="77" t="s">
         <v>69</v>
@@ -2989,7 +2986,7 @@
         <v>33</v>
       </c>
       <c r="M31" s="77" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N31" s="77" t="s">
         <v>69</v>
@@ -3035,7 +3032,7 @@
         <v>33</v>
       </c>
       <c r="M32" s="77" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N32" s="77" t="s">
         <v>69</v>
@@ -3081,7 +3078,7 @@
         <v>33</v>
       </c>
       <c r="M33" s="77" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N33" s="77" t="s">
         <v>69</v>
@@ -3127,7 +3124,7 @@
         <v>33</v>
       </c>
       <c r="M34" s="77" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N34" s="77" t="s">
         <v>69</v>
@@ -3173,7 +3170,7 @@
         <v>33</v>
       </c>
       <c r="M35" s="77" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N35" s="77" t="s">
         <v>69</v>
@@ -3219,7 +3216,7 @@
         <v>33</v>
       </c>
       <c r="M36" s="77" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N36" s="77" t="s">
         <v>69</v>
@@ -3265,7 +3262,7 @@
         <v>33</v>
       </c>
       <c r="M37" s="77" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N37" s="77" t="s">
         <v>69</v>
@@ -3311,7 +3308,7 @@
         <v>33</v>
       </c>
       <c r="M38" s="77" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N38" s="77" t="s">
         <v>69</v>
@@ -3357,7 +3354,7 @@
         <v>33</v>
       </c>
       <c r="M39" s="77" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N39" s="77" t="s">
         <v>69</v>
@@ -3403,7 +3400,7 @@
         <v>33</v>
       </c>
       <c r="M40" s="77" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N40" s="77" t="s">
         <v>69</v>
@@ -3449,7 +3446,7 @@
         <v>33</v>
       </c>
       <c r="M41" s="77" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N41" s="77" t="s">
         <v>69</v>
@@ -3466,7 +3463,7 @@
         <f>A41+1</f>
       </c>
       <c r="B42" s="77" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C42" s="78" t="s">
         <v>64</v>
@@ -3475,7 +3472,7 @@
         <v>65</v>
       </c>
       <c r="E42" s="77" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F42" s="78" t="s">
         <v>67</v>
@@ -3495,10 +3492,10 @@
         <v>33</v>
       </c>
       <c r="M42" s="77" t="s">
+        <v>81</v>
+      </c>
+      <c r="N42" s="77" t="s">
         <v>82</v>
-      </c>
-      <c r="N42" s="77" t="s">
-        <v>83</v>
       </c>
       <c r="O42" s="2"/>
       <c r="P42" s="2"/>
@@ -3512,16 +3509,16 @@
         <f>A42+1</f>
       </c>
       <c r="B43" s="77" t="s">
+        <v>83</v>
+      </c>
+      <c r="C43" s="78" t="s">
         <v>84</v>
-      </c>
-      <c r="C43" s="78" t="s">
-        <v>85</v>
       </c>
       <c r="D43" s="78" t="s">
         <v>65</v>
       </c>
       <c r="E43" s="77" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F43" s="78" t="s">
         <v>67</v>
@@ -3541,10 +3538,10 @@
         <v>33</v>
       </c>
       <c r="M43" s="77" t="s">
+        <v>81</v>
+      </c>
+      <c r="N43" s="77" t="s">
         <v>82</v>
-      </c>
-      <c r="N43" s="77" t="s">
-        <v>83</v>
       </c>
       <c r="O43" s="2"/>
       <c r="P43" s="2"/>
@@ -3558,16 +3555,16 @@
         <f>A43+1</f>
       </c>
       <c r="B44" s="77" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C44" s="78" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D44" s="78" t="s">
         <v>65</v>
       </c>
       <c r="E44" s="77" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F44" s="78" t="s">
         <v>67</v>
@@ -3587,10 +3584,10 @@
         <v>33</v>
       </c>
       <c r="M44" s="77" t="s">
+        <v>81</v>
+      </c>
+      <c r="N44" s="77" t="s">
         <v>82</v>
-      </c>
-      <c r="N44" s="77" t="s">
-        <v>83</v>
       </c>
       <c r="O44" s="2"/>
       <c r="P44" s="2"/>
@@ -3604,16 +3601,16 @@
         <f>A44+1</f>
       </c>
       <c r="B45" s="77" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C45" s="78" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D45" s="78" t="s">
         <v>65</v>
       </c>
       <c r="E45" s="77" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F45" s="78" t="s">
         <v>67</v>
@@ -3633,10 +3630,10 @@
         <v>33</v>
       </c>
       <c r="M45" s="77" t="s">
+        <v>81</v>
+      </c>
+      <c r="N45" s="77" t="s">
         <v>82</v>
-      </c>
-      <c r="N45" s="77" t="s">
-        <v>83</v>
       </c>
       <c r="O45" s="2"/>
       <c r="P45" s="2"/>
@@ -3650,7 +3647,7 @@
         <f>A45+1</f>
       </c>
       <c r="B46" s="77" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C46" s="78" t="s">
         <v>64</v>
@@ -3659,7 +3656,7 @@
         <v>65</v>
       </c>
       <c r="E46" s="77" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F46" s="78" t="s">
         <v>77</v>
@@ -3671,18 +3668,18 @@
       <c r="I46" s="81">
         <v>298</v>
       </c>
-      <c r="J46" s="82" t="s">
-        <v>78</v>
+      <c r="J46" s="82">
+        <v>50</v>
       </c>
       <c r="K46" s="83"/>
       <c r="L46" s="77" t="s">
         <v>76</v>
       </c>
       <c r="M46" s="77" t="s">
+        <v>81</v>
+      </c>
+      <c r="N46" s="77" t="s">
         <v>82</v>
-      </c>
-      <c r="N46" s="77" t="s">
-        <v>83</v>
       </c>
       <c r="O46" s="2"/>
       <c r="P46" s="2"/>
@@ -3696,16 +3693,16 @@
         <f>A46+1</f>
       </c>
       <c r="B47" s="77" t="s">
+        <v>83</v>
+      </c>
+      <c r="C47" s="78" t="s">
         <v>84</v>
-      </c>
-      <c r="C47" s="78" t="s">
-        <v>85</v>
       </c>
       <c r="D47" s="78" t="s">
         <v>65</v>
       </c>
       <c r="E47" s="77" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F47" s="78" t="s">
         <v>77</v>
@@ -3717,18 +3714,18 @@
       <c r="I47" s="81">
         <v>298</v>
       </c>
-      <c r="J47" s="82" t="s">
-        <v>78</v>
+      <c r="J47" s="82">
+        <v>50</v>
       </c>
       <c r="K47" s="83"/>
       <c r="L47" s="77" t="s">
         <v>76</v>
       </c>
       <c r="M47" s="77" t="s">
+        <v>81</v>
+      </c>
+      <c r="N47" s="77" t="s">
         <v>82</v>
-      </c>
-      <c r="N47" s="77" t="s">
-        <v>83</v>
       </c>
       <c r="O47" s="2"/>
       <c r="P47" s="2"/>
@@ -3742,16 +3739,16 @@
         <f>A47+1</f>
       </c>
       <c r="B48" s="77" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C48" s="78" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D48" s="78" t="s">
         <v>65</v>
       </c>
       <c r="E48" s="77" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F48" s="78" t="s">
         <v>75</v>
@@ -3771,10 +3768,10 @@
         <v>76</v>
       </c>
       <c r="M48" s="77" t="s">
+        <v>81</v>
+      </c>
+      <c r="N48" s="77" t="s">
         <v>82</v>
-      </c>
-      <c r="N48" s="77" t="s">
-        <v>83</v>
       </c>
       <c r="O48" s="2"/>
       <c r="P48" s="2"/>
@@ -3788,16 +3785,16 @@
         <f>A48+1</f>
       </c>
       <c r="B49" s="77" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C49" s="78" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D49" s="78" t="s">
         <v>65</v>
       </c>
       <c r="E49" s="77" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F49" s="78" t="s">
         <v>75</v>
@@ -3817,10 +3814,10 @@
         <v>76</v>
       </c>
       <c r="M49" s="77" t="s">
+        <v>81</v>
+      </c>
+      <c r="N49" s="77" t="s">
         <v>82</v>
-      </c>
-      <c r="N49" s="77" t="s">
-        <v>83</v>
       </c>
       <c r="O49" s="2"/>
       <c r="P49" s="2"/>
@@ -3834,7 +3831,7 @@
         <f>A49+1</f>
       </c>
       <c r="B50" s="77" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C50" s="78" t="s">
         <v>64</v>
@@ -3843,16 +3840,16 @@
         <v>65</v>
       </c>
       <c r="E50" s="77" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F50" s="78" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G50" s="78" t="s">
         <v>29</v>
       </c>
       <c r="H50" s="78" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I50" s="81">
         <v>298</v>
@@ -3865,10 +3862,10 @@
         <v>33</v>
       </c>
       <c r="M50" s="77" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N50" s="77" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O50" s="2"/>
       <c r="P50" s="2"/>
@@ -3882,25 +3879,25 @@
         <f>A50+1</f>
       </c>
       <c r="B51" s="77" t="s">
+        <v>83</v>
+      </c>
+      <c r="C51" s="78" t="s">
         <v>84</v>
-      </c>
-      <c r="C51" s="78" t="s">
-        <v>85</v>
       </c>
       <c r="D51" s="78" t="s">
         <v>65</v>
       </c>
       <c r="E51" s="77" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F51" s="78" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G51" s="78" t="s">
         <v>29</v>
       </c>
       <c r="H51" s="78" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I51" s="81">
         <v>298</v>
@@ -3913,10 +3910,10 @@
         <v>33</v>
       </c>
       <c r="M51" s="77" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N51" s="77" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O51" s="2"/>
       <c r="P51" s="2"/>
@@ -3930,25 +3927,25 @@
         <f>A51+1</f>
       </c>
       <c r="B52" s="77" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C52" s="78" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D52" s="78" t="s">
         <v>65</v>
       </c>
       <c r="E52" s="77" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F52" s="78" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G52" s="78" t="s">
         <v>29</v>
       </c>
       <c r="H52" s="78" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I52" s="81">
         <v>298</v>
@@ -3961,10 +3958,10 @@
         <v>33</v>
       </c>
       <c r="M52" s="77" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N52" s="77" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O52" s="2"/>
       <c r="P52" s="2"/>
@@ -3978,25 +3975,25 @@
         <f>A52+1</f>
       </c>
       <c r="B53" s="77" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C53" s="78" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D53" s="78" t="s">
         <v>65</v>
       </c>
       <c r="E53" s="77" t="s">
+        <v>89</v>
+      </c>
+      <c r="F53" s="78" t="s">
         <v>90</v>
-      </c>
-      <c r="F53" s="78" t="s">
-        <v>91</v>
       </c>
       <c r="G53" s="78" t="s">
         <v>29</v>
       </c>
       <c r="H53" s="78" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I53" s="81">
         <v>298</v>
@@ -4009,10 +4006,10 @@
         <v>33</v>
       </c>
       <c r="M53" s="77" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N53" s="77" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O53" s="2"/>
       <c r="P53" s="2"/>
@@ -4026,7 +4023,7 @@
         <f>A53+1</f>
       </c>
       <c r="B54" s="77" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C54" s="78" t="s">
         <v>64</v>
@@ -4035,16 +4032,16 @@
         <v>65</v>
       </c>
       <c r="E54" s="77" t="s">
+        <v>94</v>
+      </c>
+      <c r="F54" s="78" t="s">
         <v>95</v>
-      </c>
-      <c r="F54" s="78" t="s">
-        <v>96</v>
       </c>
       <c r="G54" s="78" t="s">
         <v>29</v>
       </c>
       <c r="H54" s="78" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I54" s="81">
         <v>298</v>
@@ -4057,10 +4054,10 @@
         <v>33</v>
       </c>
       <c r="M54" s="77" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N54" s="77" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O54" s="2"/>
       <c r="P54" s="2"/>
@@ -4074,7 +4071,7 @@
         <f>A54+1</f>
       </c>
       <c r="B55" s="77" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C55" s="78" t="s">
         <v>64</v>
@@ -4083,16 +4080,16 @@
         <v>65</v>
       </c>
       <c r="E55" s="77" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F55" s="78" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G55" s="78" t="s">
         <v>29</v>
       </c>
       <c r="H55" s="78" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I55" s="81">
         <v>298</v>
@@ -4105,10 +4102,10 @@
         <v>33</v>
       </c>
       <c r="M55" s="77" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N55" s="77" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O55" s="2"/>
       <c r="P55" s="2"/>
@@ -4122,7 +4119,7 @@
         <f>A55+1</f>
       </c>
       <c r="B56" s="77" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C56" s="78" t="s">
         <v>64</v>
@@ -4131,16 +4128,16 @@
         <v>65</v>
       </c>
       <c r="E56" s="77" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F56" s="78" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G56" s="78" t="s">
         <v>29</v>
       </c>
       <c r="H56" s="78" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I56" s="81">
         <v>298</v>
@@ -4153,10 +4150,10 @@
         <v>33</v>
       </c>
       <c r="M56" s="77" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N56" s="77" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O56" s="2"/>
       <c r="P56" s="2"/>
@@ -4170,7 +4167,7 @@
         <f>A56+1</f>
       </c>
       <c r="B57" s="77" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C57" s="78" t="s">
         <v>64</v>
@@ -4179,16 +4176,16 @@
         <v>65</v>
       </c>
       <c r="E57" s="77" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F57" s="78" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G57" s="78" t="s">
         <v>29</v>
       </c>
       <c r="H57" s="78" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I57" s="81">
         <v>298</v>
@@ -4201,10 +4198,10 @@
         <v>33</v>
       </c>
       <c r="M57" s="77" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N57" s="77" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O57" s="2"/>
       <c r="P57" s="2"/>
@@ -4218,16 +4215,16 @@
         <f>A57+1</f>
       </c>
       <c r="B58" s="77" t="s">
+        <v>102</v>
+      </c>
+      <c r="C58" s="78" t="s">
         <v>103</v>
-      </c>
-      <c r="C58" s="78" t="s">
-        <v>104</v>
       </c>
       <c r="D58" s="78" t="s">
         <v>65</v>
       </c>
       <c r="E58" s="77" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F58" s="78" t="s">
         <v>67</v>
@@ -4249,10 +4246,10 @@
         <v>33</v>
       </c>
       <c r="M58" s="77" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N58" s="77" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="O58" s="2"/>
       <c r="P58" s="2"/>
@@ -4266,16 +4263,16 @@
         <f>A58+1</f>
       </c>
       <c r="B59" s="77" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C59" s="78" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D59" s="78" t="s">
         <v>65</v>
       </c>
       <c r="E59" s="77" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F59" s="78" t="s">
         <v>67</v>
@@ -4297,10 +4294,10 @@
         <v>33</v>
       </c>
       <c r="M59" s="77" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N59" s="77" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="O59" s="2"/>
       <c r="P59" s="2"/>
@@ -4314,16 +4311,16 @@
         <f>A59+1</f>
       </c>
       <c r="B60" s="77" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C60" s="78" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D60" s="78" t="s">
         <v>65</v>
       </c>
       <c r="E60" s="77" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F60" s="78" t="s">
         <v>67</v>
@@ -4345,10 +4342,10 @@
         <v>33</v>
       </c>
       <c r="M60" s="77" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N60" s="77" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="O60" s="2"/>
       <c r="P60" s="2"/>
@@ -4362,16 +4359,16 @@
         <f>A60+1</f>
       </c>
       <c r="B61" s="77" t="s">
+        <v>102</v>
+      </c>
+      <c r="C61" s="78" t="s">
         <v>103</v>
-      </c>
-      <c r="C61" s="78" t="s">
-        <v>104</v>
       </c>
       <c r="D61" s="78" t="s">
         <v>65</v>
       </c>
       <c r="E61" s="77" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F61" s="78" t="s">
         <v>75</v>
@@ -4393,10 +4390,10 @@
         <v>76</v>
       </c>
       <c r="M61" s="77" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N61" s="77" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="O61" s="2"/>
       <c r="P61" s="2"/>
@@ -4410,16 +4407,16 @@
         <f>A61+1</f>
       </c>
       <c r="B62" s="77" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C62" s="78" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D62" s="78" t="s">
         <v>65</v>
       </c>
       <c r="E62" s="77" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F62" s="78" t="s">
         <v>75</v>
@@ -4441,10 +4438,10 @@
         <v>76</v>
       </c>
       <c r="M62" s="77" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N62" s="77" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="O62" s="2"/>
       <c r="P62" s="2"/>
@@ -4458,16 +4455,16 @@
         <f>A62+1</f>
       </c>
       <c r="B63" s="77" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C63" s="78" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D63" s="78" t="s">
         <v>65</v>
       </c>
       <c r="E63" s="77" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F63" s="78" t="s">
         <v>75</v>
@@ -4489,10 +4486,10 @@
         <v>76</v>
       </c>
       <c r="M63" s="77" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N63" s="77" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="O63" s="2"/>
       <c r="P63" s="2"/>
@@ -4506,7 +4503,7 @@
         <f>A63+1</f>
       </c>
       <c r="B64" s="77" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C64" s="78" t="s">
         <v>64</v>
@@ -4535,10 +4532,10 @@
         <v>33</v>
       </c>
       <c r="M64" s="77" t="s">
+        <v>111</v>
+      </c>
+      <c r="N64" s="77" t="s">
         <v>112</v>
-      </c>
-      <c r="N64" s="77" t="s">
-        <v>113</v>
       </c>
       <c r="O64" s="2"/>
       <c r="P64" s="2"/>
@@ -4552,16 +4549,16 @@
         <f>A64+1</f>
       </c>
       <c r="B65" s="77" t="s">
+        <v>113</v>
+      </c>
+      <c r="C65" s="78" t="s">
         <v>114</v>
-      </c>
-      <c r="C65" s="78" t="s">
-        <v>115</v>
       </c>
       <c r="D65" s="78" t="s">
         <v>65</v>
       </c>
       <c r="E65" s="77" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F65" s="78" t="s">
         <v>67</v>
@@ -4581,10 +4578,10 @@
         <v>33</v>
       </c>
       <c r="M65" s="77" t="s">
+        <v>111</v>
+      </c>
+      <c r="N65" s="77" t="s">
         <v>112</v>
-      </c>
-      <c r="N65" s="77" t="s">
-        <v>113</v>
       </c>
       <c r="O65" s="2"/>
       <c r="P65" s="2"/>
@@ -4598,16 +4595,16 @@
         <f>A65+1</f>
       </c>
       <c r="B66" s="77" t="s">
+        <v>116</v>
+      </c>
+      <c r="C66" s="78" t="s">
         <v>117</v>
-      </c>
-      <c r="C66" s="78" t="s">
-        <v>118</v>
       </c>
       <c r="D66" s="78" t="s">
         <v>65</v>
       </c>
       <c r="E66" s="77" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F66" s="78" t="s">
         <v>67</v>
@@ -4627,10 +4624,10 @@
         <v>33</v>
       </c>
       <c r="M66" s="77" t="s">
+        <v>111</v>
+      </c>
+      <c r="N66" s="77" t="s">
         <v>112</v>
-      </c>
-      <c r="N66" s="77" t="s">
-        <v>113</v>
       </c>
       <c r="O66" s="2"/>
       <c r="P66" s="2"/>
@@ -4644,16 +4641,16 @@
         <f>A66+1</f>
       </c>
       <c r="B67" s="77" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C67" s="78" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D67" s="78" t="s">
         <v>65</v>
       </c>
       <c r="E67" s="77" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F67" s="78" t="s">
         <v>67</v>
@@ -4673,10 +4670,10 @@
         <v>33</v>
       </c>
       <c r="M67" s="77" t="s">
+        <v>111</v>
+      </c>
+      <c r="N67" s="77" t="s">
         <v>112</v>
-      </c>
-      <c r="N67" s="77" t="s">
-        <v>113</v>
       </c>
       <c r="O67" s="2"/>
       <c r="P67" s="2"/>
@@ -4690,7 +4687,7 @@
         <f>A67+1</f>
       </c>
       <c r="B68" s="77" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C68" s="78" t="s">
         <v>64</v>
@@ -4702,7 +4699,7 @@
         <v>66</v>
       </c>
       <c r="F68" s="78" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G68" s="78" t="s">
         <v>29</v>
@@ -4719,10 +4716,10 @@
         <v>33</v>
       </c>
       <c r="M68" s="77" t="s">
+        <v>111</v>
+      </c>
+      <c r="N68" s="77" t="s">
         <v>112</v>
-      </c>
-      <c r="N68" s="77" t="s">
-        <v>113</v>
       </c>
       <c r="O68" s="2"/>
       <c r="P68" s="2"/>
@@ -4736,19 +4733,19 @@
         <f>A68+1</f>
       </c>
       <c r="B69" s="77" t="s">
+        <v>113</v>
+      </c>
+      <c r="C69" s="78" t="s">
         <v>114</v>
-      </c>
-      <c r="C69" s="78" t="s">
-        <v>115</v>
       </c>
       <c r="D69" s="78" t="s">
         <v>65</v>
       </c>
       <c r="E69" s="77" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F69" s="78" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G69" s="78" t="s">
         <v>29</v>
@@ -4765,10 +4762,10 @@
         <v>33</v>
       </c>
       <c r="M69" s="77" t="s">
+        <v>111</v>
+      </c>
+      <c r="N69" s="77" t="s">
         <v>112</v>
-      </c>
-      <c r="N69" s="77" t="s">
-        <v>113</v>
       </c>
       <c r="O69" s="2"/>
       <c r="P69" s="2"/>
@@ -4782,19 +4779,19 @@
         <f>A69+1</f>
       </c>
       <c r="B70" s="77" t="s">
+        <v>116</v>
+      </c>
+      <c r="C70" s="78" t="s">
         <v>117</v>
-      </c>
-      <c r="C70" s="78" t="s">
-        <v>118</v>
       </c>
       <c r="D70" s="78" t="s">
         <v>65</v>
       </c>
       <c r="E70" s="77" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F70" s="78" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G70" s="78" t="s">
         <v>29</v>
@@ -4811,10 +4808,10 @@
         <v>33</v>
       </c>
       <c r="M70" s="77" t="s">
+        <v>111</v>
+      </c>
+      <c r="N70" s="77" t="s">
         <v>112</v>
-      </c>
-      <c r="N70" s="77" t="s">
-        <v>113</v>
       </c>
       <c r="O70" s="2"/>
       <c r="P70" s="2"/>
@@ -4828,7 +4825,7 @@
         <f>A70+1</f>
       </c>
       <c r="B71" s="77" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C71" s="78" t="s">
         <v>64</v>
@@ -4857,10 +4854,10 @@
         <v>76</v>
       </c>
       <c r="M71" s="77" t="s">
+        <v>111</v>
+      </c>
+      <c r="N71" s="77" t="s">
         <v>112</v>
-      </c>
-      <c r="N71" s="77" t="s">
-        <v>113</v>
       </c>
       <c r="O71" s="2"/>
       <c r="P71" s="2"/>
@@ -4874,16 +4871,16 @@
         <f>A71+1</f>
       </c>
       <c r="B72" s="77" t="s">
+        <v>113</v>
+      </c>
+      <c r="C72" s="78" t="s">
         <v>114</v>
-      </c>
-      <c r="C72" s="78" t="s">
-        <v>115</v>
       </c>
       <c r="D72" s="78" t="s">
         <v>65</v>
       </c>
       <c r="E72" s="77" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F72" s="78" t="s">
         <v>75</v>
@@ -4903,10 +4900,10 @@
         <v>76</v>
       </c>
       <c r="M72" s="77" t="s">
+        <v>111</v>
+      </c>
+      <c r="N72" s="77" t="s">
         <v>112</v>
-      </c>
-      <c r="N72" s="77" t="s">
-        <v>113</v>
       </c>
       <c r="O72" s="2"/>
       <c r="P72" s="2"/>
@@ -4920,16 +4917,16 @@
         <f>A72+1</f>
       </c>
       <c r="B73" s="77" t="s">
+        <v>116</v>
+      </c>
+      <c r="C73" s="78" t="s">
         <v>117</v>
-      </c>
-      <c r="C73" s="78" t="s">
-        <v>118</v>
       </c>
       <c r="D73" s="78" t="s">
         <v>65</v>
       </c>
       <c r="E73" s="77" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F73" s="78" t="s">
         <v>75</v>
@@ -4949,10 +4946,10 @@
         <v>76</v>
       </c>
       <c r="M73" s="77" t="s">
+        <v>111</v>
+      </c>
+      <c r="N73" s="77" t="s">
         <v>112</v>
-      </c>
-      <c r="N73" s="77" t="s">
-        <v>113</v>
       </c>
       <c r="O73" s="2"/>
       <c r="P73" s="2"/>

</xml_diff>

<commit_message>
fixed issues with the property values
</commit_message>
<xml_diff>
--- a/carbide_expansion_april2024.xlsx
+++ b/carbide_expansion_april2024.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="167">
   <si>
     <t>Metadata</t>
   </si>
@@ -308,6 +308,9 @@
     <t>compressive yield strength</t>
   </si>
   <si>
+    <t>1512e6</t>
+  </si>
+  <si>
     <t>T3</t>
   </si>
   <si>
@@ -317,18 +320,33 @@
     <t>HfNbTaTiZr</t>
   </si>
   <si>
+    <t>929e6</t>
+  </si>
+  <si>
     <t>HfMoTaTiZr</t>
   </si>
   <si>
+    <t>1600e6</t>
+  </si>
+  <si>
     <t>HfMoNbTiZr</t>
   </si>
   <si>
+    <t>1351e6</t>
+  </si>
+  <si>
     <t>HfMoNbTaZr</t>
   </si>
   <si>
+    <t>1524e6</t>
+  </si>
+  <si>
     <t>HfMoNbTaTi</t>
   </si>
   <si>
+    <t>1369e6</t>
+  </si>
+  <si>
     <t>compressive ductility</t>
   </si>
   <si>
@@ -338,15 +356,78 @@
     <t>estimated compressive ductility</t>
   </si>
   <si>
+    <t>1007e6</t>
+  </si>
+  <si>
     <t>T4</t>
   </si>
   <si>
+    <t>535e6</t>
+  </si>
+  <si>
+    <t>1045e6</t>
+  </si>
+  <si>
+    <t>829e6</t>
+  </si>
+  <si>
+    <t>1005e6</t>
+  </si>
+  <si>
+    <t>822e6</t>
+  </si>
+  <si>
+    <t>814e6</t>
+  </si>
+  <si>
+    <t>295e6</t>
+  </si>
+  <si>
+    <t>855e6</t>
+  </si>
+  <si>
+    <t>721e6</t>
+  </si>
+  <si>
+    <t>927e6</t>
+  </si>
+  <si>
+    <t>778e6</t>
+  </si>
+  <si>
+    <t>556e6</t>
+  </si>
+  <si>
+    <t>92e6</t>
+  </si>
+  <si>
+    <t>404e6</t>
+  </si>
+  <si>
+    <t>301e6</t>
+  </si>
+  <si>
+    <t>694e6</t>
+  </si>
+  <si>
+    <t>699e6</t>
+  </si>
+  <si>
+    <t>278e6</t>
+  </si>
+  <si>
+    <t>367e6</t>
+  </si>
+  <si>
     <t xml:space="preserve">NbHfTiV </t>
   </si>
   <si>
     <t>carbide is FCC - identified to be MC-type; avg. grain size = 537e-6 meters</t>
   </si>
   <si>
+    <t>958e6</t>
+  </si>
+  <si>
     <t>F8</t>
   </si>
   <si>
@@ -362,27 +443,48 @@
     <t>carbide is FCC - identified to be MC-type,;avg. grain size = 36e-6 meters</t>
   </si>
   <si>
+    <t>1048e6</t>
+  </si>
+  <si>
     <t xml:space="preserve">NbHfTiVC0.2 </t>
   </si>
   <si>
     <t>carbide is FCC - identified to be MC-type; avg. grain size = 30e-6 meters</t>
   </si>
   <si>
+    <t>1076e6</t>
+  </si>
+  <si>
     <t>NbHfTiVC0.3</t>
   </si>
   <si>
     <t>carbide is FCC - identified to be MC-type; avg. grain size = 25e-6 meters</t>
   </si>
   <si>
+    <t>1115e6</t>
+  </si>
+  <si>
     <t>hardness</t>
   </si>
   <si>
     <t>Vickers</t>
   </si>
   <si>
+    <t>3197e6</t>
+  </si>
+  <si>
     <t>F7</t>
   </si>
   <si>
+    <t>3737e6</t>
+  </si>
+  <si>
+    <t>4021e6</t>
+  </si>
+  <si>
+    <t>4482e6</t>
+  </si>
+  <si>
     <t>Nb22.69Hf25.57Ti25.80V25.94</t>
   </si>
   <si>
@@ -392,24 +494,36 @@
     <t>nanohardness</t>
   </si>
   <si>
+    <t>8.15e9</t>
+  </si>
+  <si>
     <t>Nb25.81Hf23.80Ti22.48V25.07C2.84</t>
   </si>
   <si>
     <t xml:space="preserve">matrix phase composition of NbHfTiVC0.1  </t>
   </si>
   <si>
+    <t>7.85e9</t>
+  </si>
+  <si>
     <t>Nb24.15Hf20.54Ti26.55V26.47C2.29</t>
   </si>
   <si>
     <t xml:space="preserve">matrix phase composition of NbHfTiVC0.2  </t>
   </si>
   <si>
+    <t>7.01e9</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nb23.89Hf19.32Ti27.60V27.52C1.68 </t>
   </si>
   <si>
     <t xml:space="preserve">matrix phase composition of NbHfTiVC0.3  </t>
   </si>
   <si>
+    <t>6.94e9</t>
+  </si>
+  <si>
     <t>TiZrNbMoV</t>
   </si>
   <si>
@@ -419,6 +533,9 @@
     <t xml:space="preserve">avg. grain size = 81e-6 meters </t>
   </si>
   <si>
+    <t>2222e6</t>
+  </si>
+  <si>
     <t xml:space="preserve"> 10.1016/j.ijrmhm.2023.106547 </t>
   </si>
   <si>
@@ -428,15 +545,24 @@
     <t xml:space="preserve">avg. grain size = 33e-6 meters </t>
   </si>
   <si>
+    <t>1691e6</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ti2ZrNbMoV </t>
   </si>
   <si>
     <t xml:space="preserve">avg. grain size = 16e-6 meters </t>
   </si>
   <si>
+    <t>1588e6</t>
+  </si>
+  <si>
     <t xml:space="preserve">NbMoTaW </t>
   </si>
   <si>
+    <t>1042e6</t>
+  </si>
+  <si>
     <t>P3</t>
   </si>
   <si>
@@ -452,16 +578,31 @@
     <t>carbide is FCC; FCC phase fraction increases with carbon content</t>
   </si>
   <si>
+    <t>1285e6</t>
+  </si>
+  <si>
     <t xml:space="preserve">NbMoTaWC </t>
   </si>
   <si>
-    <t>carbide is FCC</t>
+    <t>1753e6</t>
   </si>
   <si>
     <t>(NbMoTaW)17.5C30</t>
   </si>
   <si>
+    <t>1972e6</t>
+  </si>
+  <si>
     <t>ultimate compressive strength</t>
+  </si>
+  <si>
+    <t>1059e6</t>
+  </si>
+  <si>
+    <t>2241e6</t>
+  </si>
+  <si>
+    <t>2706e6</t>
   </si>
   <si>
     <t/>
@@ -1995,18 +2136,18 @@
       <c r="I10" s="80">
         <v>298</v>
       </c>
-      <c r="J10" s="4">
-        <f>1512*10^6</f>
+      <c r="J10" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M10" s="77" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="N10" s="77" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O10" s="23"/>
       <c r="P10" s="2"/>
@@ -2020,7 +2161,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="77" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C11" s="78" t="s">
         <v>64</v>
@@ -2039,18 +2180,18 @@
       <c r="I11" s="80">
         <v>298</v>
       </c>
-      <c r="J11" s="4">
-        <f>929*10^6</f>
+      <c r="J11" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="K11" s="5"/>
       <c r="L11" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M11" s="77" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="N11" s="77" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O11" s="23"/>
       <c r="P11" s="2"/>
@@ -2064,7 +2205,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="77" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C12" s="78" t="s">
         <v>64</v>
@@ -2083,18 +2224,18 @@
       <c r="I12" s="80">
         <v>298</v>
       </c>
-      <c r="J12" s="4">
-        <f>1600*10^6</f>
+      <c r="J12" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="K12" s="5"/>
       <c r="L12" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M12" s="77" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="N12" s="77" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O12" s="81"/>
       <c r="P12" s="2"/>
@@ -2108,7 +2249,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="77" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C13" s="78" t="s">
         <v>64</v>
@@ -2127,18 +2268,18 @@
       <c r="I13" s="80">
         <v>298</v>
       </c>
-      <c r="J13" s="4">
-        <f>1351*10^6</f>
+      <c r="J13" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="K13" s="5"/>
       <c r="L13" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M13" s="77" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="N13" s="77" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O13" s="23"/>
       <c r="P13" s="2"/>
@@ -2152,7 +2293,7 @@
         <v>5</v>
       </c>
       <c r="B14" s="77" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C14" s="78" t="s">
         <v>64</v>
@@ -2171,18 +2312,18 @@
       <c r="I14" s="80">
         <v>298</v>
       </c>
-      <c r="J14" s="4">
-        <f>1524*10^6</f>
+      <c r="J14" s="4" t="s">
+        <v>77</v>
       </c>
       <c r="K14" s="5"/>
       <c r="L14" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M14" s="77" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="N14" s="77" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O14" s="23"/>
       <c r="P14" s="2"/>
@@ -2196,7 +2337,7 @@
         <v>6</v>
       </c>
       <c r="B15" s="77" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C15" s="78" t="s">
         <v>64</v>
@@ -2215,18 +2356,18 @@
       <c r="I15" s="80">
         <v>298</v>
       </c>
-      <c r="J15" s="4">
-        <f>1369*10^6</f>
+      <c r="J15" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="K15" s="5"/>
       <c r="L15" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M15" s="77" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="N15" s="77" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O15" s="23"/>
       <c r="P15" s="2"/>
@@ -2250,7 +2391,7 @@
       </c>
       <c r="E16" s="77"/>
       <c r="F16" s="78" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="G16" s="78" t="s">
         <v>29</v>
@@ -2264,13 +2405,13 @@
       </c>
       <c r="K16" s="5"/>
       <c r="L16" s="77" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="M16" s="77" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="N16" s="77" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O16" s="23"/>
       <c r="P16" s="2"/>
@@ -2284,7 +2425,7 @@
         <f>A16+1</f>
       </c>
       <c r="B17" s="77" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C17" s="78" t="s">
         <v>64</v>
@@ -2294,7 +2435,7 @@
       </c>
       <c r="E17" s="77"/>
       <c r="F17" s="78" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="G17" s="78" t="s">
         <v>29</v>
@@ -2308,13 +2449,13 @@
       </c>
       <c r="K17" s="5"/>
       <c r="L17" s="77" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="M17" s="77" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="N17" s="77" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
@@ -2328,7 +2469,7 @@
         <f>A17+1</f>
       </c>
       <c r="B18" s="77" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C18" s="78" t="s">
         <v>64</v>
@@ -2338,7 +2479,7 @@
       </c>
       <c r="E18" s="77"/>
       <c r="F18" s="78" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="G18" s="78" t="s">
         <v>29</v>
@@ -2352,13 +2493,13 @@
       </c>
       <c r="K18" s="5"/>
       <c r="L18" s="77" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="M18" s="77" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="N18" s="77" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
@@ -2372,7 +2513,7 @@
         <f>A18+1</f>
       </c>
       <c r="B19" s="77" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C19" s="78" t="s">
         <v>64</v>
@@ -2382,7 +2523,7 @@
       </c>
       <c r="E19" s="77"/>
       <c r="F19" s="78" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="G19" s="78" t="s">
         <v>29</v>
@@ -2396,13 +2537,13 @@
       </c>
       <c r="K19" s="5"/>
       <c r="L19" s="77" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="M19" s="77" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="N19" s="77" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
@@ -2416,7 +2557,7 @@
         <f>A19+1</f>
       </c>
       <c r="B20" s="77" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C20" s="78" t="s">
         <v>64</v>
@@ -2426,7 +2567,7 @@
       </c>
       <c r="E20" s="77"/>
       <c r="F20" s="78" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="G20" s="78" t="s">
         <v>29</v>
@@ -2440,13 +2581,13 @@
       </c>
       <c r="K20" s="5"/>
       <c r="L20" s="77" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="M20" s="77" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="N20" s="77" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
@@ -2460,7 +2601,7 @@
         <f>A20+1</f>
       </c>
       <c r="B21" s="77" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C21" s="78" t="s">
         <v>64</v>
@@ -2470,7 +2611,7 @@
       </c>
       <c r="E21" s="77"/>
       <c r="F21" s="78" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="G21" s="78" t="s">
         <v>29</v>
@@ -2484,13 +2625,13 @@
       </c>
       <c r="K21" s="5"/>
       <c r="L21" s="77" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="M21" s="77" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="N21" s="77" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
@@ -2523,18 +2664,18 @@
       <c r="I22" s="80">
         <v>1073</v>
       </c>
-      <c r="J22" s="4">
-        <f>1007*10^6</f>
+      <c r="J22" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="K22" s="5"/>
       <c r="L22" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M22" s="77" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="N22" s="77" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
@@ -2548,7 +2689,7 @@
         <f>A22+1</f>
       </c>
       <c r="B23" s="77" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C23" s="78" t="s">
         <v>64</v>
@@ -2567,18 +2708,18 @@
       <c r="I23" s="80">
         <v>1073</v>
       </c>
-      <c r="J23" s="4">
-        <f>535*10^6</f>
+      <c r="J23" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="K23" s="5"/>
       <c r="L23" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M23" s="77" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="N23" s="77" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
@@ -2592,7 +2733,7 @@
         <f>A23+1</f>
       </c>
       <c r="B24" s="77" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C24" s="78" t="s">
         <v>64</v>
@@ -2611,18 +2752,18 @@
       <c r="I24" s="80">
         <v>1073</v>
       </c>
-      <c r="J24" s="4">
-        <f>1045*10^6</f>
+      <c r="J24" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="K24" s="5"/>
       <c r="L24" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M24" s="77" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="N24" s="77" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
@@ -2636,7 +2777,7 @@
         <f>A24+1</f>
       </c>
       <c r="B25" s="77" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C25" s="78" t="s">
         <v>64</v>
@@ -2655,18 +2796,18 @@
       <c r="I25" s="80">
         <v>1073</v>
       </c>
-      <c r="J25" s="4">
-        <f>829*10^6</f>
+      <c r="J25" s="4" t="s">
+        <v>87</v>
       </c>
       <c r="K25" s="5"/>
       <c r="L25" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M25" s="77" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="N25" s="77" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
@@ -2680,7 +2821,7 @@
         <f>A25+1</f>
       </c>
       <c r="B26" s="77" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C26" s="78" t="s">
         <v>64</v>
@@ -2699,18 +2840,18 @@
       <c r="I26" s="80">
         <v>1073</v>
       </c>
-      <c r="J26" s="4">
-        <f>1005*10^6</f>
+      <c r="J26" s="4" t="s">
+        <v>88</v>
       </c>
       <c r="K26" s="5"/>
       <c r="L26" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M26" s="77" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="N26" s="77" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
@@ -2724,7 +2865,7 @@
         <f>A26+1</f>
       </c>
       <c r="B27" s="77" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C27" s="78" t="s">
         <v>64</v>
@@ -2743,18 +2884,18 @@
       <c r="I27" s="80">
         <v>1073</v>
       </c>
-      <c r="J27" s="4">
-        <f>822*10^6</f>
+      <c r="J27" s="4" t="s">
+        <v>89</v>
       </c>
       <c r="K27" s="5"/>
       <c r="L27" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M27" s="77" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="N27" s="77" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
@@ -2787,18 +2928,18 @@
       <c r="I28" s="80">
         <v>1273</v>
       </c>
-      <c r="J28" s="4">
-        <f>814*10^6</f>
+      <c r="J28" s="4" t="s">
+        <v>90</v>
       </c>
       <c r="K28" s="5"/>
       <c r="L28" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M28" s="77" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="N28" s="77" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O28" s="2"/>
       <c r="P28" s="2"/>
@@ -2812,7 +2953,7 @@
         <f>A28+1</f>
       </c>
       <c r="B29" s="77" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C29" s="78" t="s">
         <v>64</v>
@@ -2831,18 +2972,18 @@
       <c r="I29" s="80">
         <v>1273</v>
       </c>
-      <c r="J29" s="4">
-        <f>295*10^6</f>
+      <c r="J29" s="4" t="s">
+        <v>91</v>
       </c>
       <c r="K29" s="5"/>
       <c r="L29" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M29" s="77" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="N29" s="77" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O29" s="2"/>
       <c r="P29" s="2"/>
@@ -2856,7 +2997,7 @@
         <f>A29+1</f>
       </c>
       <c r="B30" s="77" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C30" s="78" t="s">
         <v>64</v>
@@ -2875,18 +3016,18 @@
       <c r="I30" s="80">
         <v>1273</v>
       </c>
-      <c r="J30" s="4">
-        <f>855*10^6</f>
+      <c r="J30" s="4" t="s">
+        <v>92</v>
       </c>
       <c r="K30" s="5"/>
       <c r="L30" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M30" s="77" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="N30" s="77" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O30" s="2"/>
       <c r="P30" s="2"/>
@@ -2900,7 +3041,7 @@
         <f>A30+1</f>
       </c>
       <c r="B31" s="77" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C31" s="78" t="s">
         <v>64</v>
@@ -2919,18 +3060,18 @@
       <c r="I31" s="80">
         <v>1273</v>
       </c>
-      <c r="J31" s="4">
-        <f>721*10^6</f>
+      <c r="J31" s="4" t="s">
+        <v>93</v>
       </c>
       <c r="K31" s="5"/>
       <c r="L31" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M31" s="77" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="N31" s="77" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O31" s="2"/>
       <c r="P31" s="2"/>
@@ -2944,7 +3085,7 @@
         <f>A31+1</f>
       </c>
       <c r="B32" s="77" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C32" s="78" t="s">
         <v>64</v>
@@ -2963,18 +3104,18 @@
       <c r="I32" s="80">
         <v>1273</v>
       </c>
-      <c r="J32" s="4">
-        <f>927*10^6</f>
+      <c r="J32" s="4" t="s">
+        <v>94</v>
       </c>
       <c r="K32" s="5"/>
       <c r="L32" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M32" s="77" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="N32" s="77" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O32" s="2"/>
       <c r="P32" s="2"/>
@@ -2988,7 +3129,7 @@
         <f>A32+1</f>
       </c>
       <c r="B33" s="77" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C33" s="78" t="s">
         <v>64</v>
@@ -3007,18 +3148,18 @@
       <c r="I33" s="80">
         <v>1273</v>
       </c>
-      <c r="J33" s="4">
-        <f>778*10^6</f>
+      <c r="J33" s="4" t="s">
+        <v>95</v>
       </c>
       <c r="K33" s="5"/>
       <c r="L33" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M33" s="77" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="N33" s="77" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O33" s="2"/>
       <c r="P33" s="2"/>
@@ -3051,18 +3192,18 @@
       <c r="I34" s="80">
         <v>1473</v>
       </c>
-      <c r="J34" s="4">
-        <f>556*10^6</f>
+      <c r="J34" s="4" t="s">
+        <v>96</v>
       </c>
       <c r="K34" s="5"/>
       <c r="L34" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M34" s="77" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="N34" s="77" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O34" s="2"/>
       <c r="P34" s="2"/>
@@ -3076,7 +3217,7 @@
         <f>A34+1</f>
       </c>
       <c r="B35" s="77" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C35" s="78" t="s">
         <v>64</v>
@@ -3095,18 +3236,18 @@
       <c r="I35" s="80">
         <v>1473</v>
       </c>
-      <c r="J35" s="4">
-        <f>92*10^6</f>
+      <c r="J35" s="4" t="s">
+        <v>97</v>
       </c>
       <c r="K35" s="5"/>
       <c r="L35" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M35" s="77" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="N35" s="77" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O35" s="2"/>
       <c r="P35" s="2"/>
@@ -3120,7 +3261,7 @@
         <f>A35+1</f>
       </c>
       <c r="B36" s="77" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C36" s="78" t="s">
         <v>64</v>
@@ -3139,18 +3280,18 @@
       <c r="I36" s="80">
         <v>1473</v>
       </c>
-      <c r="J36" s="4">
-        <f>404*10^6</f>
+      <c r="J36" s="4" t="s">
+        <v>98</v>
       </c>
       <c r="K36" s="5"/>
       <c r="L36" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M36" s="77" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="N36" s="77" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O36" s="2"/>
       <c r="P36" s="2"/>
@@ -3164,7 +3305,7 @@
         <f>A36+1</f>
       </c>
       <c r="B37" s="77" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C37" s="78" t="s">
         <v>64</v>
@@ -3183,18 +3324,18 @@
       <c r="I37" s="80">
         <v>1473</v>
       </c>
-      <c r="J37" s="4">
-        <f>301*10^6</f>
+      <c r="J37" s="4" t="s">
+        <v>99</v>
       </c>
       <c r="K37" s="5"/>
       <c r="L37" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M37" s="77" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="N37" s="77" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O37" s="2"/>
       <c r="P37" s="2"/>
@@ -3208,7 +3349,7 @@
         <f>A37+1</f>
       </c>
       <c r="B38" s="77" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C38" s="78" t="s">
         <v>64</v>
@@ -3227,18 +3368,18 @@
       <c r="I38" s="80">
         <v>1473</v>
       </c>
-      <c r="J38" s="4">
-        <f>694*10^6</f>
+      <c r="J38" s="4" t="s">
+        <v>100</v>
       </c>
       <c r="K38" s="5"/>
       <c r="L38" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M38" s="77" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="N38" s="77" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O38" s="2"/>
       <c r="P38" s="2"/>
@@ -3252,7 +3393,7 @@
         <f>A38+1</f>
       </c>
       <c r="B39" s="77" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C39" s="78" t="s">
         <v>64</v>
@@ -3271,18 +3412,18 @@
       <c r="I39" s="80">
         <v>1473</v>
       </c>
-      <c r="J39" s="4">
-        <f>699*10^6</f>
+      <c r="J39" s="4" t="s">
+        <v>101</v>
       </c>
       <c r="K39" s="5"/>
       <c r="L39" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M39" s="77" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="N39" s="77" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O39" s="2"/>
       <c r="P39" s="2"/>
@@ -3296,7 +3437,7 @@
         <f>A39+1</f>
       </c>
       <c r="B40" s="77" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C40" s="78" t="s">
         <v>64</v>
@@ -3315,18 +3456,18 @@
       <c r="I40" s="80">
         <v>1673</v>
       </c>
-      <c r="J40" s="4">
-        <f>278*10^6</f>
+      <c r="J40" s="4" t="s">
+        <v>102</v>
       </c>
       <c r="K40" s="5"/>
       <c r="L40" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M40" s="77" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="N40" s="77" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O40" s="2"/>
       <c r="P40" s="2"/>
@@ -3340,7 +3481,7 @@
         <f>A40+1</f>
       </c>
       <c r="B41" s="77" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C41" s="78" t="s">
         <v>64</v>
@@ -3359,18 +3500,18 @@
       <c r="I41" s="80">
         <v>1673</v>
       </c>
-      <c r="J41" s="4">
-        <f>367*10^6</f>
+      <c r="J41" s="4" t="s">
+        <v>103</v>
       </c>
       <c r="K41" s="5"/>
       <c r="L41" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M41" s="77" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="N41" s="77" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O41" s="2"/>
       <c r="P41" s="2"/>
@@ -3384,7 +3525,7 @@
         <f>A41+1</f>
       </c>
       <c r="B42" s="77" t="s">
-        <v>78</v>
+        <v>104</v>
       </c>
       <c r="C42" s="78" t="s">
         <v>64</v>
@@ -3393,7 +3534,7 @@
         <v>65</v>
       </c>
       <c r="E42" s="77" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="F42" s="78" t="s">
         <v>66</v>
@@ -3405,18 +3546,18 @@
       <c r="I42" s="80">
         <v>298</v>
       </c>
-      <c r="J42" s="4">
-        <f>958*10^6</f>
+      <c r="J42" s="4" t="s">
+        <v>106</v>
       </c>
       <c r="K42" s="5"/>
       <c r="L42" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M42" s="77" t="s">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="N42" s="77" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
       <c r="O42" s="2"/>
       <c r="P42" s="2"/>
@@ -3430,16 +3571,16 @@
         <f>A42+1</f>
       </c>
       <c r="B43" s="77" t="s">
-        <v>82</v>
+        <v>109</v>
       </c>
       <c r="C43" s="78" t="s">
-        <v>83</v>
+        <v>110</v>
       </c>
       <c r="D43" s="78" t="s">
         <v>65</v>
       </c>
       <c r="E43" s="77" t="s">
-        <v>84</v>
+        <v>111</v>
       </c>
       <c r="F43" s="78" t="s">
         <v>66</v>
@@ -3451,18 +3592,18 @@
       <c r="I43" s="80">
         <v>298</v>
       </c>
-      <c r="J43" s="4">
-        <f>1048*10^6</f>
+      <c r="J43" s="4" t="s">
+        <v>112</v>
       </c>
       <c r="K43" s="5"/>
       <c r="L43" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M43" s="77" t="s">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="N43" s="77" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
       <c r="O43" s="2"/>
       <c r="P43" s="2"/>
@@ -3476,16 +3617,16 @@
         <f>A43+1</f>
       </c>
       <c r="B44" s="77" t="s">
-        <v>85</v>
+        <v>113</v>
       </c>
       <c r="C44" s="78" t="s">
-        <v>83</v>
+        <v>110</v>
       </c>
       <c r="D44" s="78" t="s">
         <v>65</v>
       </c>
       <c r="E44" s="77" t="s">
-        <v>86</v>
+        <v>114</v>
       </c>
       <c r="F44" s="78" t="s">
         <v>66</v>
@@ -3497,18 +3638,18 @@
       <c r="I44" s="80">
         <v>298</v>
       </c>
-      <c r="J44" s="4">
-        <f>1076*10^6</f>
+      <c r="J44" s="4" t="s">
+        <v>115</v>
       </c>
       <c r="K44" s="5"/>
       <c r="L44" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M44" s="77" t="s">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="N44" s="77" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
       <c r="O44" s="2"/>
       <c r="P44" s="2"/>
@@ -3522,16 +3663,16 @@
         <f>A44+1</f>
       </c>
       <c r="B45" s="77" t="s">
-        <v>87</v>
+        <v>116</v>
       </c>
       <c r="C45" s="78" t="s">
-        <v>83</v>
+        <v>110</v>
       </c>
       <c r="D45" s="78" t="s">
         <v>65</v>
       </c>
       <c r="E45" s="77" t="s">
-        <v>88</v>
+        <v>117</v>
       </c>
       <c r="F45" s="78" t="s">
         <v>66</v>
@@ -3543,18 +3684,18 @@
       <c r="I45" s="80">
         <v>298</v>
       </c>
-      <c r="J45" s="4">
-        <f>1115*10^6</f>
+      <c r="J45" s="4" t="s">
+        <v>118</v>
       </c>
       <c r="K45" s="5"/>
       <c r="L45" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M45" s="77" t="s">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="N45" s="77" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
       <c r="O45" s="2"/>
       <c r="P45" s="2"/>
@@ -3568,7 +3709,7 @@
         <f>A45+1</f>
       </c>
       <c r="B46" s="77" t="s">
-        <v>78</v>
+        <v>104</v>
       </c>
       <c r="C46" s="78" t="s">
         <v>64</v>
@@ -3577,10 +3718,10 @@
         <v>65</v>
       </c>
       <c r="E46" s="77" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="F46" s="78" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="G46" s="78" t="s">
         <v>29</v>
@@ -3594,13 +3735,13 @@
       </c>
       <c r="K46" s="5"/>
       <c r="L46" s="77" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="M46" s="77" t="s">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="N46" s="77" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
       <c r="O46" s="2"/>
       <c r="P46" s="2"/>
@@ -3614,19 +3755,19 @@
         <f>A46+1</f>
       </c>
       <c r="B47" s="77" t="s">
-        <v>82</v>
+        <v>109</v>
       </c>
       <c r="C47" s="78" t="s">
-        <v>83</v>
+        <v>110</v>
       </c>
       <c r="D47" s="78" t="s">
         <v>65</v>
       </c>
       <c r="E47" s="77" t="s">
-        <v>84</v>
+        <v>111</v>
       </c>
       <c r="F47" s="78" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="G47" s="78" t="s">
         <v>29</v>
@@ -3640,13 +3781,13 @@
       </c>
       <c r="K47" s="5"/>
       <c r="L47" s="77" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="M47" s="77" t="s">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="N47" s="77" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
       <c r="O47" s="2"/>
       <c r="P47" s="2"/>
@@ -3660,19 +3801,19 @@
         <f>A47+1</f>
       </c>
       <c r="B48" s="77" t="s">
-        <v>85</v>
+        <v>113</v>
       </c>
       <c r="C48" s="78" t="s">
-        <v>83</v>
+        <v>110</v>
       </c>
       <c r="D48" s="78" t="s">
         <v>65</v>
       </c>
       <c r="E48" s="77" t="s">
-        <v>86</v>
+        <v>114</v>
       </c>
       <c r="F48" s="78" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="G48" s="78" t="s">
         <v>29</v>
@@ -3686,13 +3827,13 @@
       </c>
       <c r="K48" s="5"/>
       <c r="L48" s="77" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="M48" s="77" t="s">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="N48" s="77" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
       <c r="O48" s="2"/>
       <c r="P48" s="2"/>
@@ -3706,19 +3847,19 @@
         <f>A48+1</f>
       </c>
       <c r="B49" s="77" t="s">
-        <v>87</v>
+        <v>116</v>
       </c>
       <c r="C49" s="78" t="s">
-        <v>83</v>
+        <v>110</v>
       </c>
       <c r="D49" s="78" t="s">
         <v>65</v>
       </c>
       <c r="E49" s="77" t="s">
-        <v>88</v>
+        <v>117</v>
       </c>
       <c r="F49" s="78" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="G49" s="78" t="s">
         <v>29</v>
@@ -3732,13 +3873,13 @@
       </c>
       <c r="K49" s="5"/>
       <c r="L49" s="77" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="M49" s="77" t="s">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="N49" s="77" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
       <c r="O49" s="2"/>
       <c r="P49" s="2"/>
@@ -3752,7 +3893,7 @@
         <f>A49+1</f>
       </c>
       <c r="B50" s="77" t="s">
-        <v>78</v>
+        <v>104</v>
       </c>
       <c r="C50" s="78" t="s">
         <v>64</v>
@@ -3761,32 +3902,32 @@
         <v>65</v>
       </c>
       <c r="E50" s="77" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="F50" s="78" t="s">
-        <v>89</v>
+        <v>119</v>
       </c>
       <c r="G50" s="78" t="s">
         <v>29</v>
       </c>
       <c r="H50" s="78" t="s">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="I50" s="80">
         <v>298</v>
       </c>
-      <c r="J50" s="4">
-        <f>3197*10^6</f>
+      <c r="J50" s="4" t="s">
+        <v>121</v>
       </c>
       <c r="K50" s="5"/>
       <c r="L50" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M50" s="77" t="s">
-        <v>91</v>
+        <v>122</v>
       </c>
       <c r="N50" s="77" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
       <c r="O50" s="2"/>
       <c r="P50" s="2"/>
@@ -3800,41 +3941,41 @@
         <f>A50+1</f>
       </c>
       <c r="B51" s="77" t="s">
-        <v>82</v>
+        <v>109</v>
       </c>
       <c r="C51" s="78" t="s">
-        <v>83</v>
+        <v>110</v>
       </c>
       <c r="D51" s="78" t="s">
         <v>65</v>
       </c>
       <c r="E51" s="77" t="s">
-        <v>84</v>
+        <v>111</v>
       </c>
       <c r="F51" s="78" t="s">
-        <v>89</v>
+        <v>119</v>
       </c>
       <c r="G51" s="78" t="s">
         <v>29</v>
       </c>
       <c r="H51" s="78" t="s">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="I51" s="80">
         <v>298</v>
       </c>
-      <c r="J51" s="4">
-        <f>3737*10^6</f>
+      <c r="J51" s="4" t="s">
+        <v>123</v>
       </c>
       <c r="K51" s="5"/>
       <c r="L51" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M51" s="77" t="s">
-        <v>91</v>
+        <v>122</v>
       </c>
       <c r="N51" s="77" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
       <c r="O51" s="2"/>
       <c r="P51" s="2"/>
@@ -3848,41 +3989,41 @@
         <f>A51+1</f>
       </c>
       <c r="B52" s="77" t="s">
-        <v>85</v>
+        <v>113</v>
       </c>
       <c r="C52" s="78" t="s">
-        <v>83</v>
+        <v>110</v>
       </c>
       <c r="D52" s="78" t="s">
         <v>65</v>
       </c>
       <c r="E52" s="77" t="s">
-        <v>86</v>
+        <v>114</v>
       </c>
       <c r="F52" s="78" t="s">
-        <v>89</v>
+        <v>119</v>
       </c>
       <c r="G52" s="78" t="s">
         <v>29</v>
       </c>
       <c r="H52" s="78" t="s">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="I52" s="80">
         <v>298</v>
       </c>
-      <c r="J52" s="4">
-        <f>4021*10^6</f>
+      <c r="J52" s="4" t="s">
+        <v>124</v>
       </c>
       <c r="K52" s="5"/>
       <c r="L52" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M52" s="77" t="s">
-        <v>91</v>
+        <v>122</v>
       </c>
       <c r="N52" s="77" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
       <c r="O52" s="2"/>
       <c r="P52" s="2"/>
@@ -3896,41 +4037,41 @@
         <f>A52+1</f>
       </c>
       <c r="B53" s="77" t="s">
-        <v>87</v>
+        <v>116</v>
       </c>
       <c r="C53" s="78" t="s">
-        <v>83</v>
+        <v>110</v>
       </c>
       <c r="D53" s="78" t="s">
         <v>65</v>
       </c>
       <c r="E53" s="77" t="s">
-        <v>88</v>
+        <v>117</v>
       </c>
       <c r="F53" s="78" t="s">
-        <v>89</v>
+        <v>119</v>
       </c>
       <c r="G53" s="78" t="s">
         <v>29</v>
       </c>
       <c r="H53" s="78" t="s">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="I53" s="80">
         <v>298</v>
       </c>
-      <c r="J53" s="4">
-        <f>4482*10^6</f>
+      <c r="J53" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="K53" s="5"/>
       <c r="L53" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M53" s="77" t="s">
-        <v>91</v>
+        <v>122</v>
       </c>
       <c r="N53" s="77" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
       <c r="O53" s="2"/>
       <c r="P53" s="2"/>
@@ -3944,7 +4085,7 @@
         <f>A53+1</f>
       </c>
       <c r="B54" s="77" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
       <c r="C54" s="78" t="s">
         <v>64</v>
@@ -3953,32 +4094,32 @@
         <v>65</v>
       </c>
       <c r="E54" s="77" t="s">
-        <v>93</v>
+        <v>127</v>
       </c>
       <c r="F54" s="78" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
       <c r="G54" s="78" t="s">
         <v>29</v>
       </c>
       <c r="H54" s="78" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
       <c r="I54" s="80">
         <v>298</v>
       </c>
-      <c r="J54" s="4">
-        <f>8.15*10^9</f>
+      <c r="J54" s="4" t="s">
+        <v>129</v>
       </c>
       <c r="K54" s="5"/>
       <c r="L54" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M54" s="77" t="s">
-        <v>91</v>
+        <v>122</v>
       </c>
       <c r="N54" s="77" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
       <c r="O54" s="2"/>
       <c r="P54" s="2"/>
@@ -3992,7 +4133,7 @@
         <f>A54+1</f>
       </c>
       <c r="B55" s="77" t="s">
-        <v>95</v>
+        <v>130</v>
       </c>
       <c r="C55" s="78" t="s">
         <v>64</v>
@@ -4001,32 +4142,32 @@
         <v>65</v>
       </c>
       <c r="E55" s="77" t="s">
-        <v>96</v>
+        <v>131</v>
       </c>
       <c r="F55" s="78" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
       <c r="G55" s="78" t="s">
         <v>29</v>
       </c>
       <c r="H55" s="78" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
       <c r="I55" s="80">
         <v>298</v>
       </c>
-      <c r="J55" s="4">
-        <f>7.85*10^9</f>
+      <c r="J55" s="4" t="s">
+        <v>132</v>
       </c>
       <c r="K55" s="5"/>
       <c r="L55" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M55" s="77" t="s">
-        <v>91</v>
+        <v>122</v>
       </c>
       <c r="N55" s="77" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
       <c r="O55" s="2"/>
       <c r="P55" s="2"/>
@@ -4040,7 +4181,7 @@
         <f>A55+1</f>
       </c>
       <c r="B56" s="77" t="s">
-        <v>97</v>
+        <v>133</v>
       </c>
       <c r="C56" s="78" t="s">
         <v>64</v>
@@ -4049,32 +4190,32 @@
         <v>65</v>
       </c>
       <c r="E56" s="77" t="s">
-        <v>98</v>
+        <v>134</v>
       </c>
       <c r="F56" s="78" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
       <c r="G56" s="78" t="s">
         <v>29</v>
       </c>
       <c r="H56" s="78" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
       <c r="I56" s="80">
         <v>298</v>
       </c>
-      <c r="J56" s="4">
-        <f>7.01*10^9</f>
+      <c r="J56" s="4" t="s">
+        <v>135</v>
       </c>
       <c r="K56" s="5"/>
       <c r="L56" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M56" s="77" t="s">
-        <v>91</v>
+        <v>122</v>
       </c>
       <c r="N56" s="77" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
       <c r="O56" s="2"/>
       <c r="P56" s="2"/>
@@ -4088,7 +4229,7 @@
         <f>A56+1</f>
       </c>
       <c r="B57" s="77" t="s">
-        <v>99</v>
+        <v>136</v>
       </c>
       <c r="C57" s="78" t="s">
         <v>64</v>
@@ -4097,32 +4238,32 @@
         <v>65</v>
       </c>
       <c r="E57" s="77" t="s">
-        <v>100</v>
+        <v>137</v>
       </c>
       <c r="F57" s="78" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
       <c r="G57" s="78" t="s">
         <v>29</v>
       </c>
       <c r="H57" s="78" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
       <c r="I57" s="80">
         <v>298</v>
       </c>
-      <c r="J57" s="4">
-        <f>6.94*10^9</f>
+      <c r="J57" s="4" t="s">
+        <v>138</v>
       </c>
       <c r="K57" s="5"/>
       <c r="L57" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M57" s="77" t="s">
-        <v>91</v>
+        <v>122</v>
       </c>
       <c r="N57" s="77" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
       <c r="O57" s="2"/>
       <c r="P57" s="2"/>
@@ -4136,16 +4277,16 @@
         <f>A57+1</f>
       </c>
       <c r="B58" s="77" t="s">
-        <v>101</v>
+        <v>139</v>
       </c>
       <c r="C58" s="78" t="s">
-        <v>102</v>
+        <v>140</v>
       </c>
       <c r="D58" s="78" t="s">
         <v>65</v>
       </c>
       <c r="E58" s="77" t="s">
-        <v>103</v>
+        <v>141</v>
       </c>
       <c r="F58" s="78" t="s">
         <v>66</v>
@@ -4157,8 +4298,8 @@
       <c r="I58" s="80">
         <v>298</v>
       </c>
-      <c r="J58" s="4">
-        <f>2222*10^6</f>
+      <c r="J58" s="4" t="s">
+        <v>142</v>
       </c>
       <c r="K58" s="5">
         <v>50</v>
@@ -4167,10 +4308,10 @@
         <v>33</v>
       </c>
       <c r="M58" s="77" t="s">
-        <v>91</v>
+        <v>122</v>
       </c>
       <c r="N58" s="77" t="s">
-        <v>104</v>
+        <v>143</v>
       </c>
       <c r="O58" s="2"/>
       <c r="P58" s="2"/>
@@ -4184,16 +4325,16 @@
         <f>A58+1</f>
       </c>
       <c r="B59" s="77" t="s">
-        <v>105</v>
+        <v>144</v>
       </c>
       <c r="C59" s="78" t="s">
-        <v>102</v>
+        <v>140</v>
       </c>
       <c r="D59" s="78" t="s">
         <v>65</v>
       </c>
       <c r="E59" s="77" t="s">
-        <v>106</v>
+        <v>145</v>
       </c>
       <c r="F59" s="78" t="s">
         <v>66</v>
@@ -4205,8 +4346,8 @@
       <c r="I59" s="80">
         <v>298</v>
       </c>
-      <c r="J59" s="4">
-        <f>1691*10^6</f>
+      <c r="J59" s="4" t="s">
+        <v>146</v>
       </c>
       <c r="K59" s="5">
         <v>100</v>
@@ -4215,10 +4356,10 @@
         <v>33</v>
       </c>
       <c r="M59" s="77" t="s">
-        <v>91</v>
+        <v>122</v>
       </c>
       <c r="N59" s="77" t="s">
-        <v>104</v>
+        <v>143</v>
       </c>
       <c r="O59" s="2"/>
       <c r="P59" s="2"/>
@@ -4232,16 +4373,16 @@
         <f>A59+1</f>
       </c>
       <c r="B60" s="77" t="s">
-        <v>107</v>
+        <v>147</v>
       </c>
       <c r="C60" s="78" t="s">
-        <v>102</v>
+        <v>140</v>
       </c>
       <c r="D60" s="78" t="s">
         <v>65</v>
       </c>
       <c r="E60" s="77" t="s">
-        <v>108</v>
+        <v>148</v>
       </c>
       <c r="F60" s="78" t="s">
         <v>66</v>
@@ -4253,8 +4394,8 @@
       <c r="I60" s="80">
         <v>298</v>
       </c>
-      <c r="J60" s="4">
-        <f>1588*10^6</f>
+      <c r="J60" s="4" t="s">
+        <v>149</v>
       </c>
       <c r="K60" s="5">
         <v>50</v>
@@ -4263,10 +4404,10 @@
         <v>33</v>
       </c>
       <c r="M60" s="77" t="s">
-        <v>91</v>
+        <v>122</v>
       </c>
       <c r="N60" s="77" t="s">
-        <v>104</v>
+        <v>143</v>
       </c>
       <c r="O60" s="2"/>
       <c r="P60" s="2"/>
@@ -4280,19 +4421,19 @@
         <f>A60+1</f>
       </c>
       <c r="B61" s="77" t="s">
-        <v>101</v>
+        <v>139</v>
       </c>
       <c r="C61" s="78" t="s">
-        <v>102</v>
+        <v>140</v>
       </c>
       <c r="D61" s="78" t="s">
         <v>65</v>
       </c>
       <c r="E61" s="77" t="s">
-        <v>103</v>
+        <v>141</v>
       </c>
       <c r="F61" s="78" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="G61" s="78" t="s">
         <v>29</v>
@@ -4308,13 +4449,13 @@
         <v>0.5</v>
       </c>
       <c r="L61" s="77" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="M61" s="77" t="s">
-        <v>91</v>
+        <v>122</v>
       </c>
       <c r="N61" s="77" t="s">
-        <v>104</v>
+        <v>143</v>
       </c>
       <c r="O61" s="2"/>
       <c r="P61" s="2"/>
@@ -4328,19 +4469,19 @@
         <f>A61+1</f>
       </c>
       <c r="B62" s="77" t="s">
-        <v>105</v>
+        <v>144</v>
       </c>
       <c r="C62" s="78" t="s">
-        <v>102</v>
+        <v>140</v>
       </c>
       <c r="D62" s="78" t="s">
         <v>65</v>
       </c>
       <c r="E62" s="77" t="s">
-        <v>106</v>
+        <v>145</v>
       </c>
       <c r="F62" s="78" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="G62" s="78" t="s">
         <v>29</v>
@@ -4356,13 +4497,13 @@
         <v>1.5</v>
       </c>
       <c r="L62" s="77" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="M62" s="77" t="s">
-        <v>91</v>
+        <v>122</v>
       </c>
       <c r="N62" s="77" t="s">
-        <v>104</v>
+        <v>143</v>
       </c>
       <c r="O62" s="2"/>
       <c r="P62" s="2"/>
@@ -4376,19 +4517,19 @@
         <f>A62+1</f>
       </c>
       <c r="B63" s="77" t="s">
-        <v>107</v>
+        <v>147</v>
       </c>
       <c r="C63" s="78" t="s">
-        <v>102</v>
+        <v>140</v>
       </c>
       <c r="D63" s="78" t="s">
         <v>65</v>
       </c>
       <c r="E63" s="77" t="s">
-        <v>108</v>
+        <v>148</v>
       </c>
       <c r="F63" s="78" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="G63" s="78" t="s">
         <v>29</v>
@@ -4404,13 +4545,13 @@
         <v>3</v>
       </c>
       <c r="L63" s="77" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="M63" s="77" t="s">
-        <v>91</v>
+        <v>122</v>
       </c>
       <c r="N63" s="77" t="s">
-        <v>104</v>
+        <v>143</v>
       </c>
       <c r="O63" s="2"/>
       <c r="P63" s="2"/>
@@ -4424,7 +4565,7 @@
         <f>A63+1</f>
       </c>
       <c r="B64" s="77" t="s">
-        <v>109</v>
+        <v>150</v>
       </c>
       <c r="C64" s="78" t="s">
         <v>64</v>
@@ -4443,18 +4584,18 @@
       <c r="I64" s="80">
         <v>298</v>
       </c>
-      <c r="J64" s="4">
-        <f>1042*10^6</f>
+      <c r="J64" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="K64" s="5"/>
       <c r="L64" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M64" s="77" t="s">
-        <v>110</v>
+        <v>152</v>
       </c>
       <c r="N64" s="77" t="s">
-        <v>111</v>
+        <v>153</v>
       </c>
       <c r="O64" s="2"/>
       <c r="P64" s="2"/>
@@ -4468,16 +4609,16 @@
         <f>A64+1</f>
       </c>
       <c r="B65" s="77" t="s">
-        <v>112</v>
+        <v>154</v>
       </c>
       <c r="C65" s="78" t="s">
-        <v>113</v>
+        <v>155</v>
       </c>
       <c r="D65" s="78" t="s">
         <v>65</v>
       </c>
       <c r="E65" s="77" t="s">
-        <v>114</v>
+        <v>156</v>
       </c>
       <c r="F65" s="78" t="s">
         <v>66</v>
@@ -4489,18 +4630,18 @@
       <c r="I65" s="80">
         <v>298</v>
       </c>
-      <c r="J65" s="4">
-        <f>1285*10^6</f>
+      <c r="J65" s="4" t="s">
+        <v>157</v>
       </c>
       <c r="K65" s="5"/>
       <c r="L65" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M65" s="77" t="s">
-        <v>110</v>
+        <v>152</v>
       </c>
       <c r="N65" s="77" t="s">
-        <v>111</v>
+        <v>153</v>
       </c>
       <c r="O65" s="2"/>
       <c r="P65" s="2"/>
@@ -4514,16 +4655,16 @@
         <f>A65+1</f>
       </c>
       <c r="B66" s="77" t="s">
-        <v>115</v>
+        <v>158</v>
       </c>
       <c r="C66" s="78" t="s">
-        <v>83</v>
+        <v>110</v>
       </c>
       <c r="D66" s="78" t="s">
         <v>65</v>
       </c>
       <c r="E66" s="77" t="s">
-        <v>116</v>
+        <v>156</v>
       </c>
       <c r="F66" s="78" t="s">
         <v>66</v>
@@ -4535,18 +4676,18 @@
       <c r="I66" s="80">
         <v>298</v>
       </c>
-      <c r="J66" s="4">
-        <f>1753*10^6</f>
+      <c r="J66" s="4" t="s">
+        <v>159</v>
       </c>
       <c r="K66" s="5"/>
       <c r="L66" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M66" s="77" t="s">
-        <v>110</v>
+        <v>152</v>
       </c>
       <c r="N66" s="77" t="s">
-        <v>111</v>
+        <v>153</v>
       </c>
       <c r="O66" s="2"/>
       <c r="P66" s="2"/>
@@ -4560,16 +4701,16 @@
         <f>A66+1</f>
       </c>
       <c r="B67" s="77" t="s">
-        <v>117</v>
+        <v>160</v>
       </c>
       <c r="C67" s="78" t="s">
-        <v>113</v>
+        <v>155</v>
       </c>
       <c r="D67" s="78" t="s">
         <v>65</v>
       </c>
       <c r="E67" s="77" t="s">
-        <v>116</v>
+        <v>156</v>
       </c>
       <c r="F67" s="78" t="s">
         <v>66</v>
@@ -4581,18 +4722,18 @@
       <c r="I67" s="80">
         <v>298</v>
       </c>
-      <c r="J67" s="4">
-        <f>1972*10^6</f>
+      <c r="J67" s="4" t="s">
+        <v>161</v>
       </c>
       <c r="K67" s="5"/>
       <c r="L67" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M67" s="77" t="s">
-        <v>110</v>
+        <v>152</v>
       </c>
       <c r="N67" s="77" t="s">
-        <v>111</v>
+        <v>153</v>
       </c>
       <c r="O67" s="2"/>
       <c r="P67" s="2"/>
@@ -4606,7 +4747,7 @@
         <f>A67+1</f>
       </c>
       <c r="B68" s="77" t="s">
-        <v>109</v>
+        <v>150</v>
       </c>
       <c r="C68" s="78" t="s">
         <v>64</v>
@@ -4616,7 +4757,7 @@
       </c>
       <c r="E68" s="77"/>
       <c r="F68" s="78" t="s">
-        <v>118</v>
+        <v>162</v>
       </c>
       <c r="G68" s="78" t="s">
         <v>29</v>
@@ -4625,18 +4766,18 @@
       <c r="I68" s="80">
         <v>298</v>
       </c>
-      <c r="J68" s="4">
-        <f>1059*10^6</f>
+      <c r="J68" s="4" t="s">
+        <v>163</v>
       </c>
       <c r="K68" s="5"/>
       <c r="L68" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M68" s="77" t="s">
-        <v>110</v>
+        <v>152</v>
       </c>
       <c r="N68" s="77" t="s">
-        <v>111</v>
+        <v>153</v>
       </c>
       <c r="O68" s="2"/>
       <c r="P68" s="2"/>
@@ -4650,19 +4791,19 @@
         <f>A68+1</f>
       </c>
       <c r="B69" s="77" t="s">
-        <v>112</v>
+        <v>154</v>
       </c>
       <c r="C69" s="78" t="s">
-        <v>113</v>
+        <v>155</v>
       </c>
       <c r="D69" s="78" t="s">
         <v>65</v>
       </c>
       <c r="E69" s="77" t="s">
-        <v>116</v>
+        <v>156</v>
       </c>
       <c r="F69" s="78" t="s">
-        <v>118</v>
+        <v>162</v>
       </c>
       <c r="G69" s="78" t="s">
         <v>29</v>
@@ -4671,18 +4812,18 @@
       <c r="I69" s="80">
         <v>298</v>
       </c>
-      <c r="J69" s="4">
-        <f>2241*10^6</f>
+      <c r="J69" s="4" t="s">
+        <v>164</v>
       </c>
       <c r="K69" s="5"/>
       <c r="L69" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M69" s="77" t="s">
-        <v>110</v>
+        <v>152</v>
       </c>
       <c r="N69" s="77" t="s">
-        <v>111</v>
+        <v>153</v>
       </c>
       <c r="O69" s="2"/>
       <c r="P69" s="2"/>
@@ -4696,19 +4837,19 @@
         <f>A69+1</f>
       </c>
       <c r="B70" s="77" t="s">
-        <v>115</v>
+        <v>158</v>
       </c>
       <c r="C70" s="78" t="s">
-        <v>83</v>
+        <v>110</v>
       </c>
       <c r="D70" s="78" t="s">
         <v>65</v>
       </c>
       <c r="E70" s="77" t="s">
-        <v>116</v>
+        <v>156</v>
       </c>
       <c r="F70" s="78" t="s">
-        <v>118</v>
+        <v>162</v>
       </c>
       <c r="G70" s="78" t="s">
         <v>29</v>
@@ -4717,18 +4858,18 @@
       <c r="I70" s="80">
         <v>298</v>
       </c>
-      <c r="J70" s="4">
-        <f>2706*10^6</f>
+      <c r="J70" s="4" t="s">
+        <v>165</v>
       </c>
       <c r="K70" s="5"/>
       <c r="L70" s="77" t="s">
         <v>33</v>
       </c>
       <c r="M70" s="77" t="s">
-        <v>110</v>
+        <v>152</v>
       </c>
       <c r="N70" s="77" t="s">
-        <v>111</v>
+        <v>153</v>
       </c>
       <c r="O70" s="2"/>
       <c r="P70" s="2"/>
@@ -4742,7 +4883,7 @@
         <f>A70+1</f>
       </c>
       <c r="B71" s="77" t="s">
-        <v>109</v>
+        <v>150</v>
       </c>
       <c r="C71" s="78" t="s">
         <v>64</v>
@@ -4751,10 +4892,10 @@
         <v>65</v>
       </c>
       <c r="E71" s="82" t="s">
-        <v>119</v>
+        <v>166</v>
       </c>
       <c r="F71" s="78" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="G71" s="78" t="s">
         <v>29</v>
@@ -4768,13 +4909,13 @@
       </c>
       <c r="K71" s="5"/>
       <c r="L71" s="77" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="M71" s="77" t="s">
-        <v>110</v>
+        <v>152</v>
       </c>
       <c r="N71" s="77" t="s">
-        <v>111</v>
+        <v>153</v>
       </c>
       <c r="O71" s="2"/>
       <c r="P71" s="2"/>
@@ -4788,19 +4929,19 @@
         <f>A71+1</f>
       </c>
       <c r="B72" s="77" t="s">
-        <v>112</v>
+        <v>154</v>
       </c>
       <c r="C72" s="78" t="s">
-        <v>113</v>
+        <v>155</v>
       </c>
       <c r="D72" s="78" t="s">
         <v>65</v>
       </c>
       <c r="E72" s="77" t="s">
-        <v>116</v>
+        <v>156</v>
       </c>
       <c r="F72" s="78" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="G72" s="78" t="s">
         <v>29</v>
@@ -4814,13 +4955,13 @@
       </c>
       <c r="K72" s="5"/>
       <c r="L72" s="77" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="M72" s="77" t="s">
-        <v>110</v>
+        <v>152</v>
       </c>
       <c r="N72" s="77" t="s">
-        <v>111</v>
+        <v>153</v>
       </c>
       <c r="O72" s="2"/>
       <c r="P72" s="2"/>
@@ -4834,19 +4975,19 @@
         <f>A72+1</f>
       </c>
       <c r="B73" s="77" t="s">
-        <v>115</v>
+        <v>158</v>
       </c>
       <c r="C73" s="78" t="s">
-        <v>83</v>
+        <v>110</v>
       </c>
       <c r="D73" s="78" t="s">
         <v>65</v>
       </c>
       <c r="E73" s="77" t="s">
-        <v>116</v>
+        <v>156</v>
       </c>
       <c r="F73" s="78" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="G73" s="78" t="s">
         <v>29</v>
@@ -4860,13 +5001,13 @@
       </c>
       <c r="K73" s="5"/>
       <c r="L73" s="77" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="M73" s="77" t="s">
-        <v>110</v>
+        <v>152</v>
       </c>
       <c r="N73" s="77" t="s">
-        <v>111</v>
+        <v>153</v>
       </c>
       <c r="O73" s="2"/>
       <c r="P73" s="2"/>

</xml_diff>